<commit_message>
Update Fixing Import Product
</commit_message>
<xml_diff>
--- a/app/template/products_template.xlsx
+++ b/app/template/products_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\ecommerce\app\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{203530BF-C4AB-4B9F-A0AE-4454267E75B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82EB5F41-F001-4CAF-9F65-E9E79BD75603}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{CED52B4E-BC26-4E7D-AF75-41173B734B7F}"/>
   </bookViews>
@@ -36,9 +36,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
-    <t>nama</t>
-  </si>
-  <si>
     <t>category_id</t>
   </si>
   <si>
@@ -52,6 +49,9 @@
   </si>
   <si>
     <t>image</t>
+  </si>
+  <si>
+    <t>name</t>
   </si>
 </sst>
 </file>
@@ -409,7 +409,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -420,22 +420,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="57" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Add PHPSheets and Fix import product
</commit_message>
<xml_diff>
--- a/app/template/products_template.xlsx
+++ b/app/template/products_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\ecommerce\app\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82EB5F41-F001-4CAF-9F65-E9E79BD75603}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F91F8287-43E1-4C56-96CB-1D2EC1D6AFB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{CED52B4E-BC26-4E7D-AF75-41173B734B7F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{F478DACA-7646-421E-8D9C-B8FB714F195D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,22 +36,22 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>stock</t>
+  </si>
+  <si>
     <t>category_id</t>
   </si>
   <si>
-    <t>stock</t>
-  </si>
-  <si>
-    <t>price</t>
-  </si>
-  <si>
-    <t>description</t>
-  </si>
-  <si>
     <t>image</t>
-  </si>
-  <si>
-    <t>name</t>
   </si>
 </sst>
 </file>
@@ -87,8 +87,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -405,50 +408,52 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C84AF5C3-B623-427F-BC10-E73E90338D28}">
-  <dimension ref="A1:F10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F623D837-2AF0-460D-B495-09BCF0D20D65}">
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="A3" sqref="A3:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="5" width="18.140625" customWidth="1"/>
-    <col min="6" max="6" width="36.5703125" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
     </row>
-    <row r="2" spans="1:6" ht="57" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:6" ht="57" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:6" ht="57" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:6" ht="57" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:6" ht="57" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:6" ht="57" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:6" ht="57" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:6" ht="57" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:6" ht="57" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="2"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>